<commit_message>
update paragraph dan single button, untuk parenting
</commit_message>
<xml_diff>
--- a/NextgenInfo PageContent Seeding.xlsx
+++ b/NextgenInfo PageContent Seeding.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\myjpcc\nextgeninfo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12CD2CBE-3336-4AD0-B385-9A5E2AABF516}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E22EA6-A912-4867-AE7F-992A697C90C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15060" xr2:uid="{744F6DD1-6052-4E8B-B666-407797C78461}"/>
+    <workbookView xWindow="10335" yWindow="840" windowWidth="18495" windowHeight="14610" xr2:uid="{744F6DD1-6052-4E8B-B666-407797C78461}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="110">
   <si>
     <t>large</t>
   </si>
@@ -244,6 +244,123 @@
   </si>
   <si>
     <t>queue,</t>
+  </si>
+  <si>
+    <t>THE KASABLANKA</t>
+  </si>
+  <si>
+    <t>servicetimelocation</t>
+  </si>
+  <si>
+    <t>kasablankatitle1location</t>
+  </si>
+  <si>
+    <t>jpcckidskokaslocation</t>
+  </si>
+  <si>
+    <t>jpccyouthkokaslocation</t>
+  </si>
+  <si>
+    <t>jpcccampuskokaslocation</t>
+  </si>
+  <si>
+    <t>locationlocation</t>
+  </si>
+  <si>
+    <t>SERVICE TIME</t>
+  </si>
+  <si>
+    <t>LOCATION &amp; DIRECTIONS</t>
+  </si>
+  <si>
+    <t>07:15 | 9:30 | 11:45</t>
+  </si>
+  <si>
+    <t>07:15 | 9:30 | 12:45</t>
+  </si>
+  <si>
+    <t>14:00</t>
+  </si>
+  <si>
+    <t>JPCC Campus (University Students):</t>
+  </si>
+  <si>
+    <t>JPCC Youth (Grade 7-12):</t>
+  </si>
+  <si>
+    <t>JPCC Kids (Baby - Grad 6):</t>
+  </si>
+  <si>
+    <t>location2location</t>
+  </si>
+  <si>
+    <t>The Kasablanka&lt;br&gt;Mal Kota Kasablanka 3rd-4th floor&lt;br&gt;Jl. Casablanca Raya Kav. 88&lt;br&gt;Jakarta 12870</t>
+  </si>
+  <si>
+    <t>#c94</t>
+  </si>
+  <si>
+    <t>#444</t>
+  </si>
+  <si>
+    <t>linelocation</t>
+  </si>
+  <si>
+    <t>Phase Card</t>
+  </si>
+  <si>
+    <t>Parent Cue</t>
+  </si>
+  <si>
+    <t>Parent Cue merupakan materi dari bahan JPCC Kids &amp; Youth yang bisa diaplikasikan oleh orangtua di rumah. Parent Cue di desain secara khusus untuk menolong orangtua agar dapat menolong anak-anaknya dalam mengembangkan iman yang sejati. Kami akan mengirimankan Parent Cue melalui e-mail. Untuk mendapatkan Parent Cue secara berkala, klik tombol dibawah ini :</t>
+  </si>
+  <si>
+    <t>Merupakan kumpulan ringkasan singkat tentang fase, info terkait pertumbuhan &amp; perkembangan anak, tips sederhana untuk mempengaruhi pikiran dan hati mereka, mulai dari usia 0 (new baby) - SMA.</t>
+  </si>
+  <si>
+    <t>PARENT CUE</t>
+  </si>
+  <si>
+    <t>lineparenting</t>
+  </si>
+  <si>
+    <t>phasecard1parenting</t>
+  </si>
+  <si>
+    <t>phasecard2parenting</t>
+  </si>
+  <si>
+    <t>parentcue2parenting</t>
+  </si>
+  <si>
+    <t>parentcue1parenting</t>
+  </si>
+  <si>
+    <t>rgb(100, 124, 150)</t>
+  </si>
+  <si>
+    <t>#666</t>
+  </si>
+  <si>
+    <t>https://nextgen.myjpcc.org/phasecards</t>
+  </si>
+  <si>
+    <t>PHASE CARDS</t>
+  </si>
+  <si>
+    <t>https://nextgen.myjpcc.org/parentcue</t>
+  </si>
+  <si>
+    <t>110%</t>
+  </si>
+  <si>
+    <t>200%</t>
+  </si>
+  <si>
+    <t>85%</t>
+  </si>
+  <si>
+    <t>150%</t>
   </si>
 </sst>
 </file>
@@ -279,10 +396,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -597,10 +715,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E5EFF4F-6903-4312-A398-54B88C524597}">
-  <dimension ref="A2:Y10"/>
+  <dimension ref="A2:Y23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V4" sqref="V4"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Y3" sqref="Y3:Y23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,6 +729,7 @@
     <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7" customWidth="1"/>
     <col min="17" max="17" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="19.42578125" bestFit="1" customWidth="1"/>
@@ -794,7 +913,7 @@
         <v>2</v>
       </c>
       <c r="Y4" s="1" t="str">
-        <f t="shared" ref="Y4:Y10" si="0">"INSERT INTO pagecontents VALUES ("&amp;A4&amp;","&amp;B4&amp;","&amp;C4&amp;", '"&amp;D4&amp;"', "&amp;IF(E4="", "null", _xlfn.CONCAT("'", E4, "'"))&amp;", "&amp;IF(F4="", "null", _xlfn.CONCAT("'", F4, "'"))&amp;", "&amp;IF(G4="", "null", _xlfn.CONCAT("'", G4, "'"))&amp;", "&amp;IF(H4="", "null", _xlfn.CONCAT("'", H4, "'"))&amp;", "&amp;IF(I4="", "null", _xlfn.CONCAT("'", I4, "'"))&amp;", "&amp;IF(J4="", "null", _xlfn.CONCAT("'", J4, "'"))&amp;", "&amp;IF(K4="", "null", _xlfn.CONCAT("'", K4, "'"))&amp;", "&amp;IF(L4="", "null", _xlfn.CONCAT("'", L4, "'"))&amp;", "&amp;IF(M4="", "null", _xlfn.CONCAT("'", M4, "'"))&amp;", "&amp;IF(N4="", "null", _xlfn.CONCAT("'",N4, "'"))&amp;", "&amp;IF(O4="", "null", _xlfn.CONCAT("'", O4, "'"))&amp;", "&amp;IF(P4="", "null", _xlfn.CONCAT("'", P4, "'"))&amp;", "&amp;IF(Q4="", "null", _xlfn.CONCAT("'", Q4, "'"))&amp;", "&amp;IF(R4="", "null", _xlfn.CONCAT("'", R4, "'"))&amp;", "&amp;IF(S4="", "null", _xlfn.CONCAT("'", S4, "'"))&amp;", "&amp;IF(T4="", "null", _xlfn.CONCAT("'", T4, "'"))&amp;", "&amp;IF(U4="", "null", _xlfn.CONCAT("'", U4, "'"))&amp;", "&amp;IF(V4="", "null", _xlfn.CONCAT("'", V4, "'"))&amp;", "&amp;IF(W4="", "null", _xlfn.CONCAT("'", W4, "'"))&amp;", "&amp;X4&amp;", now(), now());"</f>
+        <f t="shared" ref="Y4:Y23" si="0">"INSERT INTO pagecontents VALUES ("&amp;A4&amp;","&amp;B4&amp;","&amp;C4&amp;", '"&amp;D4&amp;"', "&amp;IF(E4="", "null", _xlfn.CONCAT("'", E4, "'"))&amp;", "&amp;IF(F4="", "null", _xlfn.CONCAT("'", F4, "'"))&amp;", "&amp;IF(G4="", "null", _xlfn.CONCAT("'", G4, "'"))&amp;", "&amp;IF(H4="", "null", _xlfn.CONCAT("'", H4, "'"))&amp;", "&amp;IF(I4="", "null", _xlfn.CONCAT("'", I4, "'"))&amp;", "&amp;IF(J4="", "null", _xlfn.CONCAT("'", J4, "'"))&amp;", "&amp;IF(K4="", "null", _xlfn.CONCAT("'", K4, "'"))&amp;", "&amp;IF(L4="", "null", _xlfn.CONCAT("'", L4, "'"))&amp;", "&amp;IF(M4="", "null", _xlfn.CONCAT("'", M4, "'"))&amp;", "&amp;IF(N4="", "null", _xlfn.CONCAT("'",N4, "'"))&amp;", "&amp;IF(O4="", "null", _xlfn.CONCAT("'", O4, "'"))&amp;", "&amp;IF(P4="", "null", _xlfn.CONCAT("'", P4, "'"))&amp;", "&amp;IF(Q4="", "null", _xlfn.CONCAT("'", Q4, "'"))&amp;", "&amp;IF(R4="", "null", _xlfn.CONCAT("'", R4, "'"))&amp;", "&amp;IF(S4="", "null", _xlfn.CONCAT("'", S4, "'"))&amp;", "&amp;IF(T4="", "null", _xlfn.CONCAT("'", T4, "'"))&amp;", "&amp;IF(U4="", "null", _xlfn.CONCAT("'", U4, "'"))&amp;", "&amp;IF(V4="", "null", _xlfn.CONCAT("'", V4, "'"))&amp;", "&amp;IF(W4="", "null", _xlfn.CONCAT("'", W4, "'"))&amp;", "&amp;X4&amp;", now(), now());"</f>
         <v>INSERT INTO pagecontents VALUES (2,1,7, 'parentinghome', 'PARENTING', null, '400', '0', null, null, 'Learn more to access our Phase Cards &amp; monthly Parent Cue', null, '400', '0', null, null, '#50afdd', 'parenting-bg.jpg', 'page/parenting', 'LEARN MORE', 'large', null, null, 2, now(), now());</v>
       </c>
     </row>
@@ -1126,6 +1245,537 @@
       <c r="Y10" s="1" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO pagecontents VALUES (8,1,7, 'resourceshome', 'Resources', null, '400', '0', null, null, 'Resources for Leaders', null, '400', '0', null, null, '#34a', 'resources-bg.jpg', 'page/resources', 'LEARN MORE', 'small', null, null, 8, now(), now());</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>73</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="K11" t="s">
+        <v>71</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="M11">
+        <v>300</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11" t="s">
+        <v>88</v>
+      </c>
+      <c r="X11">
+        <v>1</v>
+      </c>
+      <c r="Y11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pagecontents VALUES (9,2,1, 'kasablankatitle1location', null, null, null, '0', null, null, 'THE KASABLANKA', '200%', '300', '0', '#c94', null, null, null, null, null, null, null, null, 1, now(), now());</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>72</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="K12" t="s">
+        <v>78</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="M12">
+        <v>100</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12" t="s">
+        <v>88</v>
+      </c>
+      <c r="X12">
+        <v>2</v>
+      </c>
+      <c r="Y12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pagecontents VALUES (10,2,1, 'servicetimelocation', null, null, null, '0', null, null, 'SERVICE TIME', '85%', '100', '0', '#c94', null, null, null, null, null, null, null, null, 2, now(), now());</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="G13">
+        <v>800</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
+        <v>89</v>
+      </c>
+      <c r="K13" t="s">
+        <v>80</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="M13">
+        <v>300</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13" t="s">
+        <v>89</v>
+      </c>
+      <c r="X13">
+        <v>3</v>
+      </c>
+      <c r="Y13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pagecontents VALUES (11,2,5, 'jpcckidskokaslocation', 'JPCC Kids (Baby - Grad 6):', '110%', '800', '0', '#444', null, '07:15 | 9:30 | 11:45', '110%', '300', '0', '#444', null, null, null, null, null, null, null, null, 3, now(), now());</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" t="s">
+        <v>84</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="G14">
+        <v>800</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14" t="s">
+        <v>89</v>
+      </c>
+      <c r="K14" t="s">
+        <v>81</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="M14">
+        <v>300</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14" t="s">
+        <v>89</v>
+      </c>
+      <c r="X14">
+        <v>4</v>
+      </c>
+      <c r="Y14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pagecontents VALUES (12,2,5, 'jpccyouthkokaslocation', 'JPCC Youth (Grade 7-12):', '110%', '800', '0', '#444', null, '07:15 | 9:30 | 12:45', '110%', '300', '0', '#444', null, null, null, null, null, null, null, null, 4, now(), now());</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" t="s">
+        <v>83</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="G15">
+        <v>800</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15" t="s">
+        <v>89</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="M15">
+        <v>300</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15" t="s">
+        <v>89</v>
+      </c>
+      <c r="X15">
+        <v>5</v>
+      </c>
+      <c r="Y15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pagecontents VALUES (13,2,5, 'jpcccampuskokaslocation', 'JPCC Campus (University Students):', '110%', '800', '0', '#444', null, '14:00', '110%', '300', '0', '#444', null, null, null, null, null, null, null, null, 5, now(), now());</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>77</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="K16" t="s">
+        <v>79</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="M16">
+        <v>100</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16" t="s">
+        <v>88</v>
+      </c>
+      <c r="X16">
+        <v>6</v>
+      </c>
+      <c r="Y16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pagecontents VALUES (14,2,1, 'locationlocation', null, null, null, '0', null, null, 'LOCATION &amp; DIRECTIONS', '85%', '100', '0', '#c94', null, null, null, null, null, null, null, null, 6, now(), now());</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>86</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="K17" t="s">
+        <v>87</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="M17">
+        <v>300</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17" t="s">
+        <v>89</v>
+      </c>
+      <c r="X17">
+        <v>7</v>
+      </c>
+      <c r="Y17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pagecontents VALUES (15,2,5, 'location2location', null, null, null, '0', null, null, 'The Kasablanka&lt;br&gt;Mal Kota Kasablanka 3rd-4th floor&lt;br&gt;Jl. Casablanca Raya Kav. 88&lt;br&gt;Jakarta 12870', '110%', '300', '0', '#444', null, null, null, null, null, null, null, null, 7, now(), now());</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>90</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="X18">
+        <v>8</v>
+      </c>
+      <c r="Y18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pagecontents VALUES (16,2,8, 'linelocation', null, null, null, '0', null, null, null, null, null, '0', null, null, null, null, null, null, null, null, null, 8, now(), now());</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>9</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>97</v>
+      </c>
+      <c r="E19" t="s">
+        <v>91</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19" t="s">
+        <v>101</v>
+      </c>
+      <c r="K19" t="s">
+        <v>94</v>
+      </c>
+      <c r="M19">
+        <v>400</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19" t="s">
+        <v>102</v>
+      </c>
+      <c r="X19">
+        <v>1</v>
+      </c>
+      <c r="Y19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pagecontents VALUES (17,9,5, 'phasecard1parenting', 'Phase Card', '150%', null, '0', 'rgb(100, 124, 150)', null, 'Merupakan kumpulan ringkasan singkat tentang fase, info terkait pertumbuhan &amp; perkembangan anak, tips sederhana untuk mempengaruhi pikiran dan hati mereka, mulai dari usia 0 (new baby) - SMA.', null, '400', '0', '#666', null, null, null, null, null, null, null, null, 1, now(), now());</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>98</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>101</v>
+      </c>
+      <c r="S20" t="s">
+        <v>103</v>
+      </c>
+      <c r="T20" t="s">
+        <v>104</v>
+      </c>
+      <c r="U20" t="s">
+        <v>0</v>
+      </c>
+      <c r="X20">
+        <v>2</v>
+      </c>
+      <c r="Y20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pagecontents VALUES (18,9,2, 'phasecard2parenting', null, null, null, '0', null, null, null, null, null, '0', null, null, 'rgb(100, 124, 150)', null, 'https://nextgen.myjpcc.org/phasecards', 'PHASE CARDS', 'large', null, null, 2, now(), now());</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>9</v>
+      </c>
+      <c r="C21">
+        <v>8</v>
+      </c>
+      <c r="D21" t="s">
+        <v>96</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="X21">
+        <v>3</v>
+      </c>
+      <c r="Y21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pagecontents VALUES (19,9,8, 'lineparenting', null, null, null, '0', null, null, null, null, null, '0', null, null, null, null, null, null, null, null, null, 3, now(), now());</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>9</v>
+      </c>
+      <c r="C22">
+        <v>5</v>
+      </c>
+      <c r="D22" t="s">
+        <v>100</v>
+      </c>
+      <c r="E22" t="s">
+        <v>92</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22" t="s">
+        <v>101</v>
+      </c>
+      <c r="K22" t="s">
+        <v>93</v>
+      </c>
+      <c r="M22">
+        <v>400</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22" t="s">
+        <v>102</v>
+      </c>
+      <c r="X22">
+        <v>4</v>
+      </c>
+      <c r="Y22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pagecontents VALUES (20,9,5, 'parentcue1parenting', 'Parent Cue', '150%', null, '0', 'rgb(100, 124, 150)', null, 'Parent Cue merupakan materi dari bahan JPCC Kids &amp; Youth yang bisa diaplikasikan oleh orangtua di rumah. Parent Cue di desain secara khusus untuk menolong orangtua agar dapat menolong anak-anaknya dalam mengembangkan iman yang sejati. Kami akan mengirimankan Parent Cue melalui e-mail. Untuk mendapatkan Parent Cue secara berkala, klik tombol dibawah ini :', null, '400', '0', '#666', null, null, null, null, null, null, null, null, 4, now(), now());</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>9</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>99</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>101</v>
+      </c>
+      <c r="S23" t="s">
+        <v>105</v>
+      </c>
+      <c r="T23" t="s">
+        <v>95</v>
+      </c>
+      <c r="U23" t="s">
+        <v>0</v>
+      </c>
+      <c r="X23">
+        <v>5</v>
+      </c>
+      <c r="Y23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO pagecontents VALUES (21,9,2, 'parentcue2parenting', null, null, null, '0', null, null, null, null, null, '0', null, null, 'rgb(100, 124, 150)', null, 'https://nextgen.myjpcc.org/parentcue', 'PARENT CUE', 'large', null, null, 5, now(), now());</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding location page from database seed
</commit_message>
<xml_diff>
--- a/NextgenInfo PageContent Seeding.xlsx
+++ b/NextgenInfo PageContent Seeding.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\myjpcc\nextgeninfo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E22EA6-A912-4867-AE7F-992A697C90C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C12D25-D831-4A05-BF5E-EFBD2A036E1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10335" yWindow="840" windowWidth="18495" windowHeight="14610" xr2:uid="{744F6DD1-6052-4E8B-B666-407797C78461}"/>
+    <workbookView xWindow="10245" yWindow="405" windowWidth="18495" windowHeight="14610" xr2:uid="{744F6DD1-6052-4E8B-B666-407797C78461}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="119">
   <si>
     <t>large</t>
   </si>
@@ -297,9 +297,6 @@
     <t>The Kasablanka&lt;br&gt;Mal Kota Kasablanka 3rd-4th floor&lt;br&gt;Jl. Casablanca Raya Kav. 88&lt;br&gt;Jakarta 12870</t>
   </si>
   <si>
-    <t>#c94</t>
-  </si>
-  <si>
     <t>#444</t>
   </si>
   <si>
@@ -357,10 +354,40 @@
     <t>200%</t>
   </si>
   <si>
-    <t>85%</t>
-  </si>
-  <si>
     <t>150%</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>servicetimelocation2</t>
+  </si>
+  <si>
+    <t>10:30 | 13:00</t>
+  </si>
+  <si>
+    <t>jpcckidsupperoomlocation</t>
+  </si>
+  <si>
+    <t>upperroomtitle1location</t>
+  </si>
+  <si>
+    <t>UPPERROOM JAKARTA</t>
+  </si>
+  <si>
+    <t>locationlocation2</t>
+  </si>
+  <si>
+    <t>location2location3</t>
+  </si>
+  <si>
+    <t>Annex Building 10th-12th floor&lt;br&gt;Wisma Nusantara Complex&lt;br&gt;Jl. M. H. Thamrin No. 59&lt;br&gt;Jakarta 10350</t>
+  </si>
+  <si>
+    <t>#e90</t>
+  </si>
+  <si>
+    <t>95%</t>
   </si>
 </sst>
 </file>
@@ -715,17 +742,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E5EFF4F-6903-4312-A398-54B88C524597}">
-  <dimension ref="A2:Y23"/>
+  <dimension ref="A2:Y28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="Y3" sqref="Y3:Y23"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="Y28" sqref="Y3:Y28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="3" width="4.5703125" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
     <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
@@ -1267,23 +1294,26 @@
         <v>71</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M11">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="N11">
         <v>0</v>
       </c>
       <c r="O11" t="s">
-        <v>88</v>
+        <v>117</v>
+      </c>
+      <c r="U11" t="s">
+        <v>0</v>
       </c>
       <c r="X11">
         <v>1</v>
       </c>
       <c r="Y11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO pagecontents VALUES (9,2,1, 'kasablankatitle1location', null, null, null, '0', null, null, 'THE KASABLANKA', '200%', '300', '0', '#c94', null, null, null, null, null, null, null, null, 1, now(), now());</v>
+        <v>INSERT INTO pagecontents VALUES (9,2,1, 'kasablankatitle1location', null, null, null, '0', null, null, 'THE KASABLANKA', '200%', '400', '0', '#e90', null, null, null, null, null, 'large', null, null, 1, now(), now());</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
@@ -1306,23 +1336,26 @@
         <v>78</v>
       </c>
       <c r="L12" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="M12">
+        <v>400</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12" t="s">
+        <v>117</v>
+      </c>
+      <c r="U12" t="s">
         <v>108</v>
-      </c>
-      <c r="M12">
-        <v>100</v>
-      </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-      <c r="O12" t="s">
-        <v>88</v>
       </c>
       <c r="X12">
         <v>2</v>
       </c>
       <c r="Y12" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO pagecontents VALUES (10,2,1, 'servicetimelocation', null, null, null, '0', null, null, 'SERVICE TIME', '85%', '100', '0', '#c94', null, null, null, null, null, null, null, null, 2, now(), now());</v>
+        <v>INSERT INTO pagecontents VALUES (10,2,1, 'servicetimelocation', null, null, null, '0', null, null, 'SERVICE TIME', '95%', '400', '0', '#e90', null, null, null, null, null, 'medium', null, null, 2, now(), now());</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
@@ -1342,7 +1375,7 @@
         <v>85</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G13">
         <v>800</v>
@@ -1351,13 +1384,13 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K13" t="s">
         <v>80</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M13">
         <v>300</v>
@@ -1366,14 +1399,17 @@
         <v>0</v>
       </c>
       <c r="O13" t="s">
-        <v>89</v>
+        <v>88</v>
+      </c>
+      <c r="U13" t="s">
+        <v>1</v>
       </c>
       <c r="X13">
         <v>3</v>
       </c>
       <c r="Y13" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO pagecontents VALUES (11,2,5, 'jpcckidskokaslocation', 'JPCC Kids (Baby - Grad 6):', '110%', '800', '0', '#444', null, '07:15 | 9:30 | 11:45', '110%', '300', '0', '#444', null, null, null, null, null, null, null, null, 3, now(), now());</v>
+        <v>INSERT INTO pagecontents VALUES (11,2,5, 'jpcckidskokaslocation', 'JPCC Kids (Baby - Grad 6):', '110%', '800', '0', '#444', null, '07:15 | 9:30 | 11:45', '110%', '300', '0', '#444', null, null, null, null, null, 'small', null, null, 3, now(), now());</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
@@ -1393,7 +1429,7 @@
         <v>84</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G14">
         <v>800</v>
@@ -1402,13 +1438,13 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K14" t="s">
         <v>81</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M14">
         <v>300</v>
@@ -1417,14 +1453,17 @@
         <v>0</v>
       </c>
       <c r="O14" t="s">
-        <v>89</v>
+        <v>88</v>
+      </c>
+      <c r="U14" t="s">
+        <v>1</v>
       </c>
       <c r="X14">
         <v>4</v>
       </c>
       <c r="Y14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO pagecontents VALUES (12,2,5, 'jpccyouthkokaslocation', 'JPCC Youth (Grade 7-12):', '110%', '800', '0', '#444', null, '07:15 | 9:30 | 12:45', '110%', '300', '0', '#444', null, null, null, null, null, null, null, null, 4, now(), now());</v>
+        <v>INSERT INTO pagecontents VALUES (12,2,5, 'jpccyouthkokaslocation', 'JPCC Youth (Grade 7-12):', '110%', '800', '0', '#444', null, '07:15 | 9:30 | 12:45', '110%', '300', '0', '#444', null, null, null, null, null, 'small', null, null, 4, now(), now());</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
@@ -1444,7 +1483,7 @@
         <v>83</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G15">
         <v>800</v>
@@ -1453,13 +1492,13 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>82</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M15">
         <v>300</v>
@@ -1468,14 +1507,17 @@
         <v>0</v>
       </c>
       <c r="O15" t="s">
-        <v>89</v>
+        <v>88</v>
+      </c>
+      <c r="U15" t="s">
+        <v>1</v>
       </c>
       <c r="X15">
         <v>5</v>
       </c>
       <c r="Y15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO pagecontents VALUES (13,2,5, 'jpcccampuskokaslocation', 'JPCC Campus (University Students):', '110%', '800', '0', '#444', null, '14:00', '110%', '300', '0', '#444', null, null, null, null, null, null, null, null, 5, now(), now());</v>
+        <v>INSERT INTO pagecontents VALUES (13,2,5, 'jpcccampuskokaslocation', 'JPCC Campus (University Students):', '110%', '800', '0', '#444', null, '14:00', '110%', '300', '0', '#444', null, null, null, null, null, 'small', null, null, 5, now(), now());</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
@@ -1498,23 +1540,26 @@
         <v>79</v>
       </c>
       <c r="L16" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="M16">
+        <v>400</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16" t="s">
+        <v>117</v>
+      </c>
+      <c r="U16" t="s">
         <v>108</v>
-      </c>
-      <c r="M16">
-        <v>100</v>
-      </c>
-      <c r="N16">
-        <v>0</v>
-      </c>
-      <c r="O16" t="s">
-        <v>88</v>
       </c>
       <c r="X16">
         <v>6</v>
       </c>
       <c r="Y16" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO pagecontents VALUES (14,2,1, 'locationlocation', null, null, null, '0', null, null, 'LOCATION &amp; DIRECTIONS', '85%', '100', '0', '#c94', null, null, null, null, null, null, null, null, 6, now(), now());</v>
+        <v>INSERT INTO pagecontents VALUES (14,2,1, 'locationlocation', null, null, null, '0', null, null, 'LOCATION &amp; DIRECTIONS', '95%', '400', '0', '#e90', null, null, null, null, null, 'medium', null, null, 6, now(), now());</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
@@ -1537,7 +1582,7 @@
         <v>87</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M17">
         <v>300</v>
@@ -1546,14 +1591,17 @@
         <v>0</v>
       </c>
       <c r="O17" t="s">
-        <v>89</v>
+        <v>88</v>
+      </c>
+      <c r="U17" t="s">
+        <v>1</v>
       </c>
       <c r="X17">
         <v>7</v>
       </c>
       <c r="Y17" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO pagecontents VALUES (15,2,5, 'location2location', null, null, null, '0', null, null, 'The Kasablanka&lt;br&gt;Mal Kota Kasablanka 3rd-4th floor&lt;br&gt;Jl. Casablanca Raya Kav. 88&lt;br&gt;Jakarta 12870', '110%', '300', '0', '#444', null, null, null, null, null, null, null, null, 7, now(), now());</v>
+        <v>INSERT INTO pagecontents VALUES (15,2,5, 'location2location', null, null, null, '0', null, null, 'The Kasablanka&lt;br&gt;Mal Kota Kasablanka 3rd-4th floor&lt;br&gt;Jl. Casablanca Raya Kav. 88&lt;br&gt;Jakarta 12870', '110%', '300', '0', '#444', null, null, null, null, null, 'small', null, null, 7, now(), now());</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
@@ -1567,7 +1615,7 @@
         <v>8</v>
       </c>
       <c r="D18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -1594,31 +1642,31 @@
         <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H19">
         <v>0</v>
       </c>
       <c r="I19" t="s">
+        <v>100</v>
+      </c>
+      <c r="K19" t="s">
+        <v>93</v>
+      </c>
+      <c r="M19">
+        <v>400</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19" t="s">
         <v>101</v>
-      </c>
-      <c r="K19" t="s">
-        <v>94</v>
-      </c>
-      <c r="M19">
-        <v>400</v>
-      </c>
-      <c r="N19">
-        <v>0</v>
-      </c>
-      <c r="O19" t="s">
-        <v>102</v>
       </c>
       <c r="X19">
         <v>1</v>
@@ -1639,7 +1687,7 @@
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -1648,13 +1696,13 @@
         <v>0</v>
       </c>
       <c r="Q20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="S20" t="s">
+        <v>102</v>
+      </c>
+      <c r="T20" t="s">
         <v>103</v>
-      </c>
-      <c r="T20" t="s">
-        <v>104</v>
       </c>
       <c r="U20" t="s">
         <v>0</v>
@@ -1678,7 +1726,7 @@
         <v>8</v>
       </c>
       <c r="D21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H21">
         <v>0</v>
@@ -1705,31 +1753,31 @@
         <v>5</v>
       </c>
       <c r="D22" t="s">
+        <v>99</v>
+      </c>
+      <c r="E22" t="s">
+        <v>91</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22" t="s">
         <v>100</v>
       </c>
-      <c r="E22" t="s">
+      <c r="K22" t="s">
         <v>92</v>
       </c>
-      <c r="F22" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22" t="s">
+      <c r="M22">
+        <v>400</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22" t="s">
         <v>101</v>
-      </c>
-      <c r="K22" t="s">
-        <v>93</v>
-      </c>
-      <c r="M22">
-        <v>400</v>
-      </c>
-      <c r="N22">
-        <v>0</v>
-      </c>
-      <c r="O22" t="s">
-        <v>102</v>
       </c>
       <c r="X22">
         <v>4</v>
@@ -1750,7 +1798,7 @@
         <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -1759,13 +1807,13 @@
         <v>0</v>
       </c>
       <c r="Q23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="S23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="T23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="U23" t="s">
         <v>0</v>
@@ -1776,6 +1824,228 @@
       <c r="Y23" s="1" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO pagecontents VALUES (21,9,2, 'parentcue2parenting', null, null, null, '0', null, null, null, null, null, '0', null, null, 'rgb(100, 124, 150)', null, 'https://nextgen.myjpcc.org/parentcue', 'PARENT CUE', 'large', null, null, 5, now(), now());</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>112</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="K24" t="s">
+        <v>113</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="M24">
+        <v>400</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24" t="s">
+        <v>117</v>
+      </c>
+      <c r="U24" t="s">
+        <v>0</v>
+      </c>
+      <c r="X24">
+        <v>1</v>
+      </c>
+      <c r="Y24" s="1" t="str">
+        <f t="shared" ref="Y24:Y25" si="1">"INSERT INTO pagecontents VALUES ("&amp;A24&amp;","&amp;B24&amp;","&amp;C24&amp;", '"&amp;D24&amp;"', "&amp;IF(E24="", "null", _xlfn.CONCAT("'", E24, "'"))&amp;", "&amp;IF(F24="", "null", _xlfn.CONCAT("'", F24, "'"))&amp;", "&amp;IF(G24="", "null", _xlfn.CONCAT("'", G24, "'"))&amp;", "&amp;IF(H24="", "null", _xlfn.CONCAT("'", H24, "'"))&amp;", "&amp;IF(I24="", "null", _xlfn.CONCAT("'", I24, "'"))&amp;", "&amp;IF(J24="", "null", _xlfn.CONCAT("'", J24, "'"))&amp;", "&amp;IF(K24="", "null", _xlfn.CONCAT("'", K24, "'"))&amp;", "&amp;IF(L24="", "null", _xlfn.CONCAT("'", L24, "'"))&amp;", "&amp;IF(M24="", "null", _xlfn.CONCAT("'", M24, "'"))&amp;", "&amp;IF(N24="", "null", _xlfn.CONCAT("'",N24, "'"))&amp;", "&amp;IF(O24="", "null", _xlfn.CONCAT("'", O24, "'"))&amp;", "&amp;IF(P24="", "null", _xlfn.CONCAT("'", P24, "'"))&amp;", "&amp;IF(Q24="", "null", _xlfn.CONCAT("'", Q24, "'"))&amp;", "&amp;IF(R24="", "null", _xlfn.CONCAT("'", R24, "'"))&amp;", "&amp;IF(S24="", "null", _xlfn.CONCAT("'", S24, "'"))&amp;", "&amp;IF(T24="", "null", _xlfn.CONCAT("'", T24, "'"))&amp;", "&amp;IF(U24="", "null", _xlfn.CONCAT("'", U24, "'"))&amp;", "&amp;IF(V24="", "null", _xlfn.CONCAT("'", V24, "'"))&amp;", "&amp;IF(W24="", "null", _xlfn.CONCAT("'", W24, "'"))&amp;", "&amp;X24&amp;", now(), now());"</f>
+        <v>INSERT INTO pagecontents VALUES (22,2,1, 'upperroomtitle1location', null, null, null, '0', null, null, 'UPPERROOM JAKARTA', '200%', '400', '0', '#e90', null, null, null, null, null, 'large', null, null, 1, now(), now());</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>109</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="K25" t="s">
+        <v>78</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="M25">
+        <v>400</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25" t="s">
+        <v>117</v>
+      </c>
+      <c r="U25" t="s">
+        <v>108</v>
+      </c>
+      <c r="X25">
+        <v>2</v>
+      </c>
+      <c r="Y25" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO pagecontents VALUES (23,2,1, 'servicetimelocation2', null, null, null, '0', null, null, 'SERVICE TIME', '95%', '400', '0', '#e90', null, null, null, null, null, 'medium', null, null, 2, now(), now());</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>5</v>
+      </c>
+      <c r="D26" t="s">
+        <v>111</v>
+      </c>
+      <c r="E26" t="s">
+        <v>85</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="G26">
+        <v>800</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26" t="s">
+        <v>88</v>
+      </c>
+      <c r="K26" t="s">
+        <v>110</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="M26">
+        <v>300</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26" t="s">
+        <v>88</v>
+      </c>
+      <c r="U26" t="s">
+        <v>1</v>
+      </c>
+      <c r="X26">
+        <v>3</v>
+      </c>
+      <c r="Y26" s="1" t="str">
+        <f t="shared" ref="Y26:Y28" si="2">"INSERT INTO pagecontents VALUES ("&amp;A26&amp;","&amp;B26&amp;","&amp;C26&amp;", '"&amp;D26&amp;"', "&amp;IF(E26="", "null", _xlfn.CONCAT("'", E26, "'"))&amp;", "&amp;IF(F26="", "null", _xlfn.CONCAT("'", F26, "'"))&amp;", "&amp;IF(G26="", "null", _xlfn.CONCAT("'", G26, "'"))&amp;", "&amp;IF(H26="", "null", _xlfn.CONCAT("'", H26, "'"))&amp;", "&amp;IF(I26="", "null", _xlfn.CONCAT("'", I26, "'"))&amp;", "&amp;IF(J26="", "null", _xlfn.CONCAT("'", J26, "'"))&amp;", "&amp;IF(K26="", "null", _xlfn.CONCAT("'", K26, "'"))&amp;", "&amp;IF(L26="", "null", _xlfn.CONCAT("'", L26, "'"))&amp;", "&amp;IF(M26="", "null", _xlfn.CONCAT("'", M26, "'"))&amp;", "&amp;IF(N26="", "null", _xlfn.CONCAT("'",N26, "'"))&amp;", "&amp;IF(O26="", "null", _xlfn.CONCAT("'", O26, "'"))&amp;", "&amp;IF(P26="", "null", _xlfn.CONCAT("'", P26, "'"))&amp;", "&amp;IF(Q26="", "null", _xlfn.CONCAT("'", Q26, "'"))&amp;", "&amp;IF(R26="", "null", _xlfn.CONCAT("'", R26, "'"))&amp;", "&amp;IF(S26="", "null", _xlfn.CONCAT("'", S26, "'"))&amp;", "&amp;IF(T26="", "null", _xlfn.CONCAT("'", T26, "'"))&amp;", "&amp;IF(U26="", "null", _xlfn.CONCAT("'", U26, "'"))&amp;", "&amp;IF(V26="", "null", _xlfn.CONCAT("'", V26, "'"))&amp;", "&amp;IF(W26="", "null", _xlfn.CONCAT("'", W26, "'"))&amp;", "&amp;X26&amp;", now(), now());"</f>
+        <v>INSERT INTO pagecontents VALUES (24,2,5, 'jpcckidsupperoomlocation', 'JPCC Kids (Baby - Grad 6):', '110%', '800', '0', '#444', null, '10:30 | 13:00', '110%', '300', '0', '#444', null, null, null, null, null, 'small', null, null, 3, now(), now());</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>114</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="K27" t="s">
+        <v>79</v>
+      </c>
+      <c r="L27" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="M27">
+        <v>400</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27" t="s">
+        <v>117</v>
+      </c>
+      <c r="U27" t="s">
+        <v>108</v>
+      </c>
+      <c r="X27">
+        <v>6</v>
+      </c>
+      <c r="Y27" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO pagecontents VALUES (25,2,1, 'locationlocation2', null, null, null, '0', null, null, 'LOCATION &amp; DIRECTIONS', '95%', '400', '0', '#e90', null, null, null, null, null, 'medium', null, null, 6, now(), now());</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
+      <c r="D28" t="s">
+        <v>115</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="K28" t="s">
+        <v>116</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="M28">
+        <v>300</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28" t="s">
+        <v>88</v>
+      </c>
+      <c r="U28" t="s">
+        <v>1</v>
+      </c>
+      <c r="X28">
+        <v>7</v>
+      </c>
+      <c r="Y28" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO pagecontents VALUES (26,2,5, 'location2location3', null, null, null, '0', null, null, 'Annex Building 10th-12th floor&lt;br&gt;Wisma Nusantara Complex&lt;br&gt;Jl. M. H. Thamrin No. 59&lt;br&gt;Jakarta 10350', '110%', '300', '0', '#444', null, null, null, null, null, 'small', null, null, 7, now(), now());</v>
       </c>
     </row>
   </sheetData>

</xml_diff>